<commit_message>
final code with comment
tut 6
</commit_message>
<xml_diff>
--- a/tut06/output/2001CB02.xlsx
+++ b/tut06/output/2001CB02.xlsx
@@ -511,10 +511,10 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -526,10 +526,10 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -550,10 +550,10 @@
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -574,10 +574,10 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -610,7 +610,7 @@
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -634,7 +634,7 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -658,7 +658,7 @@
         <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -670,10 +670,10 @@
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -706,7 +706,7 @@
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -730,7 +730,7 @@
         <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -742,10 +742,10 @@
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -775,10 +775,10 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -799,10 +799,10 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -826,7 +826,7 @@
         <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -838,10 +838,10 @@
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
@@ -871,10 +871,10 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>